<commit_message>
更新 test_請求管理_駐車場別請求一覧 Signed-off-by: MaHongTao <mht@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_請求管理/test_請求管理_駐車場別請求一覧.xlsx
+++ b/test_請求管理/test_請求管理_駐車場別請求一覧.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="13650" tabRatio="758" activeTab="1"/>
+    <workbookView windowWidth="27765" windowHeight="13650" tabRatio="758" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798">
   <si>
     <t>SQL</t>
   </si>
@@ -2445,44 +2445,20 @@
   <si>
     <t>004-001-025</t>
   </si>
-  <si>
-    <t>004-001-026</t>
-  </si>
-  <si>
-    <t>004-001-027</t>
-  </si>
-  <si>
-    <t>004-001-028</t>
-  </si>
-  <si>
-    <t>004-001-029</t>
-  </si>
-  <si>
-    <t>004-001-030</t>
-  </si>
-  <si>
-    <t>004-001-031</t>
-  </si>
-  <si>
-    <t>004-001-032</t>
-  </si>
-  <si>
-    <t>004-001-033</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ \¥* #,##0_ ;_ \¥* \-#,##0_ ;_ \¥* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="48">
     <font>
@@ -2597,67 +2573,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2666,43 +2581,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -2725,17 +2603,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2751,7 +2642,30 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2765,9 +2679,26 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2783,16 +2714,56 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="ＭＳ ゴシック"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -2800,8 +2771,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="ＭＳ ゴシック"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2898,7 +2874,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2922,30 +3018,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2953,102 +3025,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3077,60 +3053,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -3145,8 +3067,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3169,23 +3091,77 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="34" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3198,179 +3174,179 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="178" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="41" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3378,13 +3354,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -3394,28 +3370,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
-    <xf numFmtId="38" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
-    <xf numFmtId="38" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -3578,11 +3554,11 @@
     <cellStyle name="40% - 强调文字颜色 6" xfId="61" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="62" builtinId="52"/>
     <cellStyle name="Comma [0]" xfId="63"/>
-    <cellStyle name="超链接 2" xfId="64"/>
-    <cellStyle name="Comma [0] 3 2" xfId="65"/>
+    <cellStyle name="Comma [0] 3 2" xfId="64"/>
+    <cellStyle name="超链接 2" xfId="65"/>
     <cellStyle name="Currency [0] 2" xfId="66"/>
-    <cellStyle name="常规 2 4" xfId="67"/>
-    <cellStyle name="Normal_Sheet1" xfId="68"/>
+    <cellStyle name="Normal_Sheet1" xfId="67"/>
+    <cellStyle name="常规 2 4" xfId="68"/>
     <cellStyle name="ハイパーリンク 2" xfId="69"/>
     <cellStyle name="ハイパーリンク 2 3" xfId="70"/>
     <cellStyle name="標準 2 2 3" xfId="71"/>
@@ -3597,8 +3573,8 @@
     <cellStyle name="標準 4" xfId="80"/>
     <cellStyle name="標準 4 2" xfId="81"/>
     <cellStyle name="標準 4 3" xfId="82"/>
-    <cellStyle name="超链接 4" xfId="83"/>
-    <cellStyle name="標準 4 3 2" xfId="84"/>
+    <cellStyle name="標準 4 3 2" xfId="83"/>
+    <cellStyle name="超链接 4" xfId="84"/>
     <cellStyle name="標準 5" xfId="85"/>
     <cellStyle name="標準_Sheet1" xfId="86"/>
     <cellStyle name="常规 2" xfId="87"/>
@@ -3972,7 +3948,7 @@
   <dimension ref="A1:IE192"/>
   <sheetViews>
     <sheetView topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="A163" sqref="$A163:$XFD194"/>
+      <selection activeCell="E195" sqref="E195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -15788,7 +15764,7 @@
   <sheetPr/>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K45" sqref="H42 K45"/>
     </sheetView>
   </sheetViews>
@@ -16787,8 +16763,8 @@
   <sheetPr/>
   <dimension ref="B2:BY54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -16889,45 +16865,29 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B10" s="9" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="11" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B11" s="9" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="12" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B12" s="9" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B13" s="9" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B14" s="9" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="15" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B15" s="9" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B16" s="9" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="1" ht="12" spans="2:2">
-      <c r="B17" s="9" t="s">
-        <v>805</v>
-      </c>
+    <row r="10" s="1" customFormat="1" spans="2:2">
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="2:2">
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="2:2">
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="2:2">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="2:2">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="2:2">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="2:2">
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="2:2">
+      <c r="B17" s="9"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="12"/>
     <row r="19" s="1" customFormat="1" ht="12"/>

</xml_diff>